<commit_message>
Atualizacão da pagina dados financeiros
</commit_message>
<xml_diff>
--- a/Pegada de Carbono Report.xlsx
+++ b/Pegada de Carbono Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://muvamozorg-my.sharepoint.com/personal/janio_muianga_muvamoz_org/Documents/Departamento MIS/PROJECTOS/SISTEMA DE MONITORIA/PAM VERDE/Dashboard_Empreendedorismo_Versão1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_1BB4223F8C1E2C4FD647F310C7B2DF9959492C7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FE7DA15-360D-4A19-98F5-6F17C66B9440}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="11_1BB4223F8C1E2C4FD647F310C7B2DF9959492C7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EECA2848-4981-44DE-901B-46A121829E38}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Pecada_de_Carbono_Report" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pecada_de_Carbono_Report!$G$1:$G$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Pecada_de_Carbono_Report!$D$1:$D$113</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -909,7 +909,7 @@
   <dimension ref="A1:AF113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G106" sqref="G106:G113"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1253,7 @@
         <v>33</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>68</v>
+        <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>35</v>
@@ -12023,7 +12023,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="G1:G113" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="D1:D113" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>